<commit_message>
bouton de la page produit
</commit_message>
<xml_diff>
--- a/Soutenance/Template+de+Plan+de+tests.xlsx
+++ b/Soutenance/Template+de+Plan+de+tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Script_fetch" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t xml:space="preserve">Fichier JS</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">la fonction doit retourner l’ensemble des valeurs contenues dans la page produit correspond à apiLink. Si cela fonctionne cela les envoie dans la fonction index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier si les données affichées correspondent à celles du serveur</t>
   </si>
   <si>
     <t xml:space="preserve">s’il n’y a pas de data, un message est affiché dans la console.</t>
@@ -168,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -210,12 +213,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -272,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,11 +302,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,13 +385,13 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
@@ -489,9 +482,11 @@
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -499,22 +494,24 @@
         <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -5503,13 +5500,13 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
@@ -5589,19 +5586,19 @@
     </row>
     <row r="4" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -5609,14 +5606,14 @@
       <c r="B5" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -5624,14 +5621,14 @@
       <c r="B6" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>29</v>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -5639,14 +5636,14 @@
       <c r="B7" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>32</v>
+      <c r="C7" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -5654,14 +5651,14 @@
       <c r="B8" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>34</v>
+      <c r="C8" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="7"/>
     </row>
@@ -5669,34 +5666,34 @@
       <c r="B9" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>37</v>
+      <c r="C9" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C10" s="9" t="s">
-        <v>39</v>
+      <c r="C10" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="9" t="s">
-        <v>40</v>
+      <c r="C11" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C12" s="9" t="s">
-        <v>41</v>
+      <c r="C12" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -5704,16 +5701,16 @@
     </row>
     <row r="13" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>